<commit_message>
MOSIP-221 updated storage size excel document
</commit_message>
<xml_diff>
--- a/docs/_sources/hardware_sizing/MOSIP_Storage_Estimate-v1.1.xlsx
+++ b/docs/_sources/hardware_sizing/MOSIP_Storage_Estimate-v1.1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1045452\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1045452\Documents\GitHub\documentation\docs\_sources\hardware_sizing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF010ACB-E0DB-4C21-8888-D59B0B59119A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B311FFAD-F0E7-456F-8924-57603F37D7CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{1EC5AC42-BAD7-4A03-8494-5044B1627450}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="1" xr2:uid="{1EC5AC42-BAD7-4A03-8494-5044B1627450}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="66">
   <si>
     <t>Value</t>
   </si>
@@ -240,12 +240,24 @@
   <si>
     <t>Documents size in MB*</t>
   </si>
+  <si>
+    <t>This document is useful for calculating the storage size of database &amp; file system (HDFS or CEPH) requiered for running MOSIP. Countries can use this document to estimate their storage requierment when they install MOSIP.</t>
+  </si>
+  <si>
+    <t>Revision History</t>
+  </si>
+  <si>
+    <t>22nd June 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Document Created for MOSIP Release: 1.1 </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,6 +307,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -405,7 +425,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -440,9 +460,27 @@
     <xf numFmtId="2" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -452,29 +490,23 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -790,10 +822,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C820EB-2114-4115-856F-33DCB8B3520D}">
-  <dimension ref="B2:L20"/>
+  <dimension ref="B2:L23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:L20"/>
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -810,284 +842,335 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-    </row>
-    <row r="4" spans="2:12" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="B4" s="6" t="s">
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B3" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+    </row>
+    <row r="6" spans="2:12" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="B6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F6" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="I6" s="14" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B5" s="7" t="s">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B7" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C7" s="8">
         <v>100000000</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F7" s="10">
         <f>Calculations!C20</f>
         <v>214576.72119140625</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H7" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I7" s="10">
         <f>Calculations!C55</f>
         <v>512695.3125</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B6" s="7" t="s">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B8" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C8" s="7">
         <v>3</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E8" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F8" s="10">
         <f>Calculations!F20</f>
         <v>571366.67892336845</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H8" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I8" s="10">
         <f>Calculations!F55</f>
         <v>2197265.625</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B7" s="7" t="s">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B9" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C9" s="7">
         <v>20</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E9" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F9" s="10">
         <f>Calculations!I20</f>
         <v>3353.8788557052612</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H9" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I9" s="10">
         <f>Calculations!I55</f>
         <v>659179.6875</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B8" s="7" t="s">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B10" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C10" s="7">
         <v>5</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E10" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F10" s="10">
         <f>Calculations!L20</f>
         <v>23720.785975456238</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="11">
-        <f>SUM(I5:I7)</f>
+      <c r="I10" s="11">
+        <f>SUM(I7:I9)</f>
         <v>3369140.625</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B9" s="7" t="s">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B11" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C11" s="7">
         <v>20</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F11" s="10">
         <f>Calculations!C39</f>
         <v>3777.4443626403809</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B10" s="16" t="s">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B12" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C12" s="12">
         <v>0.25</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E12" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F12" s="10">
         <f>Calculations!F39</f>
         <v>5308.5498511791229</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B11" s="16" t="s">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B13" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C13" s="12">
         <v>0.25</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F13" s="10">
         <f>Calculations!I39</f>
         <v>8.8289380073547363</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B12" s="16" t="s">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B14" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C14" s="12">
         <v>0.25</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E14" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F14" s="10">
         <f>Calculations!L39</f>
         <v>2015.0095224380493</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B13" s="16" t="s">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B15" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C15" s="12">
         <v>1.5</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="11">
-        <f>SUM(F5:F12)</f>
+      <c r="F15" s="11">
+        <f>SUM(F7:F14)</f>
         <v>824127.89762020111</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B14" s="16" t="s">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B16" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C16" s="12">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B16" s="20" t="s">
+    <row r="18" spans="2:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="27"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="22"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B22" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="25"/>
+      <c r="L22" s="25"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B23" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="K23" s="24"/>
+      <c r="L23" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="6">
+    <mergeCell ref="B23:I23"/>
+    <mergeCell ref="J23:L23"/>
     <mergeCell ref="B2:L2"/>
-    <mergeCell ref="B16:L20"/>
+    <mergeCell ref="B3:L4"/>
+    <mergeCell ref="B18:L20"/>
+    <mergeCell ref="B22:L22"/>
   </mergeCells>
-  <conditionalFormatting sqref="F5:F12">
+  <conditionalFormatting sqref="F7:F14">
     <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="min"/>
@@ -1101,7 +1184,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:I7">
+  <conditionalFormatting sqref="I7:I9">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -1129,7 +1212,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F5:F12</xm:sqref>
+          <xm:sqref>F7:F14</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{1EA89635-5B66-49C8-B08A-B2F7F5B9D35F}">
@@ -1140,7 +1223,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I5:I7</xm:sqref>
+          <xm:sqref>I7:I9</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1152,8 +1235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79E5495B-9988-45B7-9D98-7487AFB47652}">
   <dimension ref="B2:P55"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.35"/>
@@ -1180,40 +1263,40 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
     </row>
     <row r="4" spans="2:16" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="15"/>
+      <c r="C4" s="21"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="15"/>
+      <c r="F4" s="21"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="I4" s="15"/>
+      <c r="I4" s="21"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="13" t="s">
+      <c r="K4" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="L4" s="13"/>
+      <c r="L4" s="19"/>
       <c r="P4" s="2"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.35">
@@ -1273,28 +1356,28 @@
         <v>13</v>
       </c>
       <c r="C7" s="4">
-        <f>Summary!$C$5*Summary!C6*50</f>
+        <f>Summary!$C$7*Summary!C8*50</f>
         <v>15000000000</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F7" s="4">
-        <f>Summary!C5</f>
+        <f>Summary!C7</f>
         <v>100000000</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I7" s="4">
-        <f>Summary!$C$5*Summary!$C$9</f>
+        <f>Summary!$C$7*Summary!$C$11</f>
         <v>2000000000</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="L7" s="4">
-        <f>Summary!$C$5*Summary!C6</f>
+        <f>Summary!$C$7*Summary!C8</f>
         <v>300000000</v>
       </c>
     </row>
@@ -1371,7 +1454,7 @@
         <v>16</v>
       </c>
       <c r="F11" s="4">
-        <f>Summary!$C$5*Summary!$C$7*Summary!$C$8</f>
+        <f>Summary!$C$7*Summary!$C$9*Summary!$C$10</f>
         <v>10000000000</v>
       </c>
       <c r="H11" s="3" t="s">
@@ -1384,7 +1467,7 @@
         <v>16</v>
       </c>
       <c r="L11" s="4">
-        <f>Summary!$C$5*Summary!$C$6*20</f>
+        <f>Summary!$C$7*Summary!$C$8*20</f>
         <v>6000000000</v>
       </c>
     </row>
@@ -1473,7 +1556,7 @@
         <v>19</v>
       </c>
       <c r="L15" s="4">
-        <f>Summary!$C$5*Summary!$C$6</f>
+        <f>Summary!$C$7*Summary!$C$8</f>
         <v>300000000</v>
       </c>
     </row>
@@ -1604,25 +1687,25 @@
       </c>
     </row>
     <row r="23" spans="2:16" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="15"/>
+      <c r="C23" s="21"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="14" t="s">
+      <c r="E23" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="F23" s="15"/>
+      <c r="F23" s="21"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="14" t="s">
+      <c r="H23" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="I23" s="15"/>
+      <c r="I23" s="21"/>
       <c r="J23" s="2"/>
-      <c r="K23" s="13" t="s">
+      <c r="K23" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="L23" s="13"/>
+      <c r="L23" s="19"/>
       <c r="P23" s="2"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.35">
@@ -1682,14 +1765,14 @@
         <v>13</v>
       </c>
       <c r="C26" s="4">
-        <f>Summary!$C$5*Summary!$C$6</f>
+        <f>Summary!$C$7*Summary!$C$8</f>
         <v>300000000</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F26" s="4">
-        <f>Summary!$C$5</f>
+        <f>Summary!$C$7</f>
         <v>100000000</v>
       </c>
       <c r="H26" s="3" t="s">
@@ -1702,7 +1785,7 @@
         <v>13</v>
       </c>
       <c r="L26" s="4">
-        <f>Summary!$C$5</f>
+        <f>Summary!$C$7</f>
         <v>100000000</v>
       </c>
     </row>
@@ -1779,7 +1862,7 @@
         <v>16</v>
       </c>
       <c r="F30" s="4">
-        <f>Summary!C5*Summary!C7*50%</f>
+        <f>Summary!C7*Summary!C9*50%</f>
         <v>1000000000</v>
       </c>
       <c r="H30" s="3" t="s">
@@ -1792,7 +1875,7 @@
         <v>16</v>
       </c>
       <c r="L30" s="4">
-        <f>Summary!$C$5</f>
+        <f>Summary!$C$7</f>
         <v>100000000</v>
       </c>
     </row>
@@ -1863,7 +1946,7 @@
         <v>19</v>
       </c>
       <c r="C34" s="4">
-        <f>Summary!$C$5/10</f>
+        <f>Summary!$C$7/10</f>
         <v>10000000</v>
       </c>
       <c r="E34" s="3" t="s">
@@ -2014,110 +2097,110 @@
       </c>
     </row>
     <row r="42" spans="2:12" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="B42" s="13" t="s">
+      <c r="B42" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C42" s="13"/>
-      <c r="E42" s="13" t="s">
+      <c r="C42" s="19"/>
+      <c r="E42" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="F42" s="13"/>
-      <c r="H42" s="13" t="s">
+      <c r="F42" s="19"/>
+      <c r="H42" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="I42" s="13"/>
-      <c r="K42" s="13" t="s">
+      <c r="I42" s="19"/>
+      <c r="K42" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="L42" s="13"/>
+      <c r="L42" s="19"/>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B43" s="18" t="s">
+      <c r="B43" s="13" t="s">
         <v>41</v>
       </c>
       <c r="C43" s="3">
         <v>0</v>
       </c>
-      <c r="E43" s="18" t="s">
+      <c r="E43" s="13" t="s">
         <v>41</v>
       </c>
       <c r="F43" s="3">
-        <f>Summary!C10</f>
+        <f>Summary!C12</f>
         <v>0.25</v>
       </c>
-      <c r="H43" s="18" t="s">
+      <c r="H43" s="13" t="s">
         <v>41</v>
       </c>
       <c r="I43" s="3">
-        <f>Summary!C10</f>
+        <f>Summary!C12</f>
         <v>0.25</v>
       </c>
-      <c r="K43" s="17" t="s">
+      <c r="K43" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L43" s="17"/>
+      <c r="L43" s="18"/>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B44" s="18" t="s">
+      <c r="B44" s="13" t="s">
         <v>43</v>
       </c>
       <c r="C44" s="3">
         <v>0</v>
       </c>
-      <c r="E44" s="18" t="s">
+      <c r="E44" s="13" t="s">
         <v>43</v>
       </c>
       <c r="F44" s="3">
-        <f>Summary!C11</f>
+        <f>Summary!C13</f>
         <v>0.25</v>
       </c>
-      <c r="H44" s="18" t="s">
+      <c r="H44" s="13" t="s">
         <v>43</v>
       </c>
       <c r="I44" s="3">
-        <f>Summary!C11</f>
+        <f>Summary!C13</f>
         <v>0.25</v>
       </c>
-      <c r="K44" s="17"/>
-      <c r="L44" s="17"/>
+      <c r="K44" s="18"/>
+      <c r="L44" s="18"/>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B45" s="18" t="s">
+      <c r="B45" s="13" t="s">
         <v>40</v>
       </c>
       <c r="C45" s="3">
         <v>0</v>
       </c>
-      <c r="E45" s="18" t="s">
+      <c r="E45" s="13" t="s">
         <v>40</v>
       </c>
       <c r="F45" s="3">
-        <f>Summary!C12</f>
+        <f>Summary!C14</f>
         <v>0.25</v>
       </c>
-      <c r="H45" s="18" t="s">
+      <c r="H45" s="13" t="s">
         <v>40</v>
       </c>
       <c r="I45" s="3">
-        <f>Summary!C12</f>
+        <f>Summary!C14</f>
         <v>0.25</v>
       </c>
-      <c r="K45" s="17"/>
-      <c r="L45" s="17"/>
+      <c r="K45" s="18"/>
+      <c r="L45" s="18"/>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B46" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C46" s="3">
-        <f>Summary!C13</f>
+        <f>Summary!C15</f>
         <v>1.5</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>24</v>
       </c>
       <c r="F46" s="3">
-        <f>Summary!C13</f>
+        <f>Summary!C15</f>
         <v>1.5</v>
       </c>
       <c r="H46" s="3" t="s">
@@ -2126,8 +2209,8 @@
       <c r="I46" s="3">
         <v>0</v>
       </c>
-      <c r="K46" s="17"/>
-      <c r="L46" s="17"/>
+      <c r="K46" s="18"/>
+      <c r="L46" s="18"/>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B47" s="3" t="s">
@@ -2148,8 +2231,8 @@
       <c r="I47" s="3">
         <v>0</v>
       </c>
-      <c r="K47" s="17"/>
-      <c r="L47" s="17"/>
+      <c r="K47" s="18"/>
+      <c r="L47" s="18"/>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B48" s="3"/>
@@ -2158,8 +2241,8 @@
       <c r="F48" s="3"/>
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
-      <c r="K48" s="17"/>
-      <c r="L48" s="17"/>
+      <c r="K48" s="18"/>
+      <c r="L48" s="18"/>
     </row>
     <row r="49" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B49" s="3" t="s">
@@ -2183,8 +2266,8 @@
         <f>I43+I44+I45+I46+I47</f>
         <v>0.75</v>
       </c>
-      <c r="K49" s="17"/>
-      <c r="L49" s="17"/>
+      <c r="K49" s="18"/>
+      <c r="L49" s="18"/>
     </row>
     <row r="50" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B50" s="3"/>
@@ -2193,33 +2276,33 @@
       <c r="F50" s="3"/>
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
-      <c r="K50" s="17"/>
-      <c r="L50" s="17"/>
+      <c r="K50" s="18"/>
+      <c r="L50" s="18"/>
     </row>
     <row r="51" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B51" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C51" s="3">
-        <f>Summary!$C$5*C49</f>
+        <f>Summary!$C$7*C49</f>
         <v>175000000</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>37</v>
       </c>
       <c r="F51" s="3">
-        <f>Summary!$C$5*Summary!$C$6*F49</f>
+        <f>Summary!$C$7*Summary!$C$8*F49</f>
         <v>750000000</v>
       </c>
       <c r="H51" s="3" t="s">
         <v>37</v>
       </c>
       <c r="I51" s="3">
-        <f>Summary!$C$5*Summary!$C$6*I49</f>
+        <f>Summary!$C$7*Summary!$C$8*I49</f>
         <v>225000000</v>
       </c>
-      <c r="K51" s="17"/>
-      <c r="L51" s="17"/>
+      <c r="K51" s="18"/>
+      <c r="L51" s="18"/>
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B52" s="3" t="s">
@@ -2243,8 +2326,8 @@
         <f>I51/1024</f>
         <v>219726.5625</v>
       </c>
-      <c r="K52" s="17"/>
-      <c r="L52" s="17"/>
+      <c r="K52" s="18"/>
+      <c r="L52" s="18"/>
     </row>
     <row r="53" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B53" s="3"/>
@@ -2253,33 +2336,33 @@
       <c r="F53" s="3"/>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
-      <c r="K53" s="17"/>
-      <c r="L53" s="17"/>
+      <c r="K53" s="18"/>
+      <c r="L53" s="18"/>
     </row>
     <row r="54" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B54" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C54" s="3">
-        <f>Summary!C14</f>
+        <f>Summary!C16</f>
         <v>3</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>42</v>
       </c>
       <c r="F54" s="3">
-        <f>Summary!C14</f>
+        <f>Summary!C16</f>
         <v>3</v>
       </c>
       <c r="H54" s="3" t="s">
         <v>42</v>
       </c>
       <c r="I54" s="3">
-        <f>Summary!C14</f>
+        <f>Summary!C16</f>
         <v>3</v>
       </c>
-      <c r="K54" s="17"/>
-      <c r="L54" s="17"/>
+      <c r="K54" s="18"/>
+      <c r="L54" s="18"/>
     </row>
     <row r="55" spans="2:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B55" s="5" t="s">
@@ -2303,8 +2386,8 @@
         <f>I52*I54</f>
         <v>659179.6875</v>
       </c>
-      <c r="K55" s="22"/>
-      <c r="L55" s="23"/>
+      <c r="K55" s="16"/>
+      <c r="L55" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="15">

</xml_diff>

<commit_message>
updated lable in estimate calculator
</commit_message>
<xml_diff>
--- a/docs/_sources/hardware_sizing/MOSIP_Storage_Estimate-v1.1.xlsx
+++ b/docs/_sources/hardware_sizing/MOSIP_Storage_Estimate-v1.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1045452\Documents\GitHub\documentation\docs\_sources\hardware_sizing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2F77B3-08B3-4BC2-919F-DCAF3091329D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69230D7-929A-4B2B-83CC-70BFE1F48EAB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{1EC5AC42-BAD7-4A03-8494-5044B1627450}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="91">
   <si>
     <t>Value</t>
   </si>
@@ -211,9 +211,6 @@
   </si>
   <si>
     <t>Data Size in KB</t>
-  </si>
-  <si>
-    <t>Size (GB) After Archive</t>
   </si>
   <si>
     <t>File System Storage</t>
@@ -323,6 +320,12 @@
   </si>
   <si>
     <t>We have revisited the ddatabase sizing and updated the document for MOSIP Release: 1.1 with in depth assumptions</t>
+  </si>
+  <si>
+    <t>Live data size (GB) after archival</t>
+  </si>
+  <si>
+    <t>Live data size (GB) without archival</t>
   </si>
 </sst>
 </file>
@@ -854,6 +857,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -869,9 +890,6 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -883,21 +901,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1246,63 +1249,63 @@
   <dimension ref="B2:L56"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B57" sqref="B57"/>
+      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.1796875" customWidth="1"/>
     <col min="2" max="2" width="43.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.36328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:12" s="1" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="B2" s="51" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
+      <c r="B2" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
     </row>
     <row r="3" spans="2:12" s="7" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="50" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
+      <c r="B3" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
     </row>
     <row r="4" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
     </row>
     <row r="5" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B5" s="44"/>
@@ -1318,19 +1321,19 @@
       <c r="L5" s="44"/>
     </row>
     <row r="6" spans="2:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="52" t="s">
-        <v>88</v>
-      </c>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
-      <c r="H6" s="53"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="53"/>
-      <c r="L6" s="54"/>
+      <c r="B6" s="57" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="58"/>
+      <c r="L6" s="59"/>
     </row>
     <row r="7" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H7" s="7"/>
@@ -1353,7 +1356,7 @@
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B9" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" s="19">
         <v>100000000</v>
@@ -1393,7 +1396,7 @@
     </row>
     <row r="14" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B14" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C14" s="16">
         <v>75</v>
@@ -1401,7 +1404,7 @@
     </row>
     <row r="15" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B15" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C15" s="16">
         <v>365</v>
@@ -1409,7 +1412,7 @@
     </row>
     <row r="16" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B16" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C16" s="16">
         <v>95</v>
@@ -1421,19 +1424,19 @@
     </row>
     <row r="18" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B18" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>59</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>56</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.35">
@@ -1540,7 +1543,7 @@
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B26" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C26" s="18">
         <v>50</v>
@@ -1552,7 +1555,7 @@
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B27" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C27" s="18">
         <v>30</v>
@@ -1564,7 +1567,7 @@
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B28" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C28" s="18">
         <v>20</v>
@@ -1576,7 +1579,7 @@
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B29" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C29" s="18">
         <v>10</v>
@@ -1598,25 +1601,25 @@
     </row>
     <row r="31" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="32" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B32" s="45" t="s">
-        <v>63</v>
-      </c>
-      <c r="C32" s="46"/>
-      <c r="D32" s="47"/>
-      <c r="F32" s="48" t="s">
-        <v>61</v>
-      </c>
-      <c r="G32" s="49"/>
+      <c r="B32" s="51" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="52"/>
+      <c r="D32" s="53"/>
+      <c r="F32" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="G32" s="55"/>
     </row>
     <row r="33" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B33" s="26" t="s">
         <v>24</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="D33" s="27" t="s">
-        <v>60</v>
+        <v>89</v>
       </c>
       <c r="F33" s="37" t="s">
         <v>20</v>
@@ -1824,7 +1827,7 @@
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B47" s="32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C47" s="8">
         <v>1.25</v>
@@ -1847,45 +1850,45 @@
       </c>
     </row>
     <row r="50" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B50" s="50" t="s">
-        <v>83</v>
-      </c>
-      <c r="C50" s="50"/>
-      <c r="D50" s="50"/>
-      <c r="E50" s="50"/>
-      <c r="F50" s="50"/>
-      <c r="G50" s="50"/>
-      <c r="H50" s="50"/>
-      <c r="I50" s="50"/>
-      <c r="J50" s="50"/>
-      <c r="K50" s="50"/>
-      <c r="L50" s="50"/>
+      <c r="B50" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="C50" s="45"/>
+      <c r="D50" s="45"/>
+      <c r="E50" s="45"/>
+      <c r="F50" s="45"/>
+      <c r="G50" s="45"/>
+      <c r="H50" s="45"/>
+      <c r="I50" s="45"/>
+      <c r="J50" s="45"/>
+      <c r="K50" s="45"/>
+      <c r="L50" s="45"/>
     </row>
     <row r="51" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B51" s="50"/>
-      <c r="C51" s="50"/>
-      <c r="D51" s="50"/>
-      <c r="E51" s="50"/>
-      <c r="F51" s="50"/>
-      <c r="G51" s="50"/>
-      <c r="H51" s="50"/>
-      <c r="I51" s="50"/>
-      <c r="J51" s="50"/>
-      <c r="K51" s="50"/>
-      <c r="L51" s="50"/>
+      <c r="B51" s="45"/>
+      <c r="C51" s="45"/>
+      <c r="D51" s="45"/>
+      <c r="E51" s="45"/>
+      <c r="F51" s="45"/>
+      <c r="G51" s="45"/>
+      <c r="H51" s="45"/>
+      <c r="I51" s="45"/>
+      <c r="J51" s="45"/>
+      <c r="K51" s="45"/>
+      <c r="L51" s="45"/>
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B52" s="50"/>
-      <c r="C52" s="50"/>
-      <c r="D52" s="50"/>
-      <c r="E52" s="50"/>
-      <c r="F52" s="50"/>
-      <c r="G52" s="50"/>
-      <c r="H52" s="50"/>
-      <c r="I52" s="50"/>
-      <c r="J52" s="50"/>
-      <c r="K52" s="50"/>
-      <c r="L52" s="50"/>
+      <c r="B52" s="45"/>
+      <c r="C52" s="45"/>
+      <c r="D52" s="45"/>
+      <c r="E52" s="45"/>
+      <c r="F52" s="45"/>
+      <c r="G52" s="45"/>
+      <c r="H52" s="45"/>
+      <c r="I52" s="45"/>
+      <c r="J52" s="45"/>
+      <c r="K52" s="45"/>
+      <c r="L52" s="45"/>
     </row>
     <row r="53" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B53" s="43"/>
@@ -1901,67 +1904,67 @@
       <c r="L53" s="43"/>
     </row>
     <row r="54" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B54" s="55" t="s">
+      <c r="B54" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="C54" s="46"/>
+      <c r="D54" s="46"/>
+      <c r="E54" s="46"/>
+      <c r="F54" s="46"/>
+      <c r="G54" s="46"/>
+      <c r="H54" s="46"/>
+      <c r="I54" s="46"/>
+      <c r="J54" s="46"/>
+      <c r="K54" s="46"/>
+      <c r="L54" s="46"/>
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B55" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="C55" s="47"/>
+      <c r="D55" s="47"/>
+      <c r="E55" s="47"/>
+      <c r="F55" s="47"/>
+      <c r="G55" s="47"/>
+      <c r="H55" s="47"/>
+      <c r="I55" s="47"/>
+      <c r="J55" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="C54" s="55"/>
-      <c r="D54" s="55"/>
-      <c r="E54" s="55"/>
-      <c r="F54" s="55"/>
-      <c r="G54" s="55"/>
-      <c r="H54" s="55"/>
-      <c r="I54" s="55"/>
-      <c r="J54" s="55"/>
-      <c r="K54" s="55"/>
-      <c r="L54" s="55"/>
-    </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B55" s="56" t="s">
+      <c r="K55" s="47"/>
+      <c r="L55" s="47"/>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B56" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="C56" s="49"/>
+      <c r="D56" s="49"/>
+      <c r="E56" s="49"/>
+      <c r="F56" s="49"/>
+      <c r="G56" s="49"/>
+      <c r="H56" s="49"/>
+      <c r="I56" s="50"/>
+      <c r="J56" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="C55" s="56"/>
-      <c r="D55" s="56"/>
-      <c r="E55" s="56"/>
-      <c r="F55" s="56"/>
-      <c r="G55" s="56"/>
-      <c r="H55" s="56"/>
-      <c r="I55" s="56"/>
-      <c r="J55" s="56" t="s">
-        <v>85</v>
-      </c>
-      <c r="K55" s="56"/>
-      <c r="L55" s="56"/>
-    </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B56" s="57" t="s">
-        <v>89</v>
-      </c>
-      <c r="C56" s="58"/>
-      <c r="D56" s="58"/>
-      <c r="E56" s="58"/>
-      <c r="F56" s="58"/>
-      <c r="G56" s="58"/>
-      <c r="H56" s="58"/>
-      <c r="I56" s="59"/>
-      <c r="J56" s="57" t="s">
-        <v>87</v>
-      </c>
-      <c r="K56" s="58"/>
-      <c r="L56" s="59"/>
+      <c r="K56" s="49"/>
+      <c r="L56" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="B3:L4"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B6:L6"/>
     <mergeCell ref="B50:L52"/>
     <mergeCell ref="B54:L54"/>
     <mergeCell ref="B55:I55"/>
     <mergeCell ref="J55:L55"/>
     <mergeCell ref="B56:I56"/>
     <mergeCell ref="J56:L56"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="B3:L4"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="B6:L6"/>
   </mergeCells>
   <conditionalFormatting sqref="C34:C45">
     <cfRule type="dataBar" priority="3">
@@ -2082,19 +2085,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="B2" s="51" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
+      <c r="B2" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
     </row>
     <row r="4" spans="2:16" ht="18.5" x14ac:dyDescent="0.35">
       <c r="B4" s="60" t="s">
@@ -2483,27 +2486,27 @@
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B20" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C20" s="3">
         <v>0</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F20" s="24">
         <f>((F9*F10*F11)/1024/1024/1024)*75%</f>
         <v>2793.9677238464355</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I20" s="24">
         <f>((I5*I6*I7)/1024/1024/1024)*25%</f>
         <v>48.894435167312622</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L20" s="24">
         <f>((L9*L10*L11)/1024/1024/1024)*75%</f>
@@ -2512,28 +2515,28 @@
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B21" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C21" s="13">
         <f>(C19-C20)</f>
         <v>2.4121254682540894</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F21" s="13">
         <f>(F19-F20)</f>
         <v>12165.885418653488</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I21" s="13">
         <f>(I19-I20)</f>
         <v>147.05583453178406</v>
       </c>
       <c r="K21" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L21" s="13">
         <f>(L19-L20)</f>
@@ -2953,27 +2956,27 @@
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B41" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C41" s="24">
         <f>((C29*C30*C31)/1024/1024/1024)*75%</f>
         <v>942.964106798172</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F41" s="24">
         <f>((F29*F30*F31)/1024/1024/1024)*75%</f>
         <v>523.86894822120667</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I41" s="24">
         <v>0</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L41" s="24">
         <f>((L25*L26*L27)/1024/1024/1024)*50%</f>
@@ -2982,28 +2985,28 @@
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B42" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C42" s="13">
         <f>(C40-C41)</f>
         <v>1152.9773473739624</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F42" s="13">
         <f>(F40-F41)</f>
         <v>454.04769480228424</v>
       </c>
       <c r="H42" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I42" s="13">
         <f>(I40-I41)</f>
         <v>61.700120568275452</v>
       </c>
       <c r="K42" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L42" s="13">
         <f>(L40-L41)</f>
@@ -3414,28 +3417,28 @@
     </row>
     <row r="62" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B62" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C62" s="24">
         <f>C61*95%</f>
         <v>7431.9541454315186</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F62" s="24">
         <f>F61*95%</f>
         <v>2229.5862436294556</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I62" s="24">
         <f>I61*95%</f>
         <v>10404.735803604126</v>
       </c>
       <c r="K62" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L62" s="24">
         <f>L61*95%</f>
@@ -3444,28 +3447,28 @@
     </row>
     <row r="63" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B63" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C63" s="13">
         <f>(C61-C62)</f>
         <v>391.15548133850098</v>
       </c>
       <c r="E63" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F63" s="13">
         <f>(F61-F62)</f>
         <v>117.34664440155029</v>
       </c>
       <c r="H63" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I63" s="13">
         <f>(I61-I62)</f>
         <v>547.61767387390137</v>
       </c>
       <c r="K63" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L63" s="13">
         <f>(L61-L62)</f>
@@ -3474,19 +3477,19 @@
     </row>
     <row r="66" spans="2:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B66" s="68" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C66" s="69"/>
       <c r="E66" s="68" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F66" s="69"/>
       <c r="H66" s="68" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I66" s="69"/>
       <c r="K66" s="68" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L66" s="69"/>
     </row>
@@ -3756,11 +3759,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="K45:L45"/>
-    <mergeCell ref="K67:L78"/>
     <mergeCell ref="B2:L2"/>
     <mergeCell ref="B66:C66"/>
     <mergeCell ref="B4:C4"/>
@@ -3774,6 +3772,11 @@
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="K45:L45"/>
+    <mergeCell ref="K67:L78"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>